<commit_message>
asp book project ex
</commit_message>
<xml_diff>
--- a/PLAN_Workflow.xlsx
+++ b/PLAN_Workflow.xlsx
@@ -113,14 +113,6 @@
   </si>
   <si>
     <t>10
-(314-323)</t>
-  </si>
-  <si>
-    <t>10
-(324-333)</t>
-  </si>
-  <si>
-    <t>10
 (334-343)</t>
   </si>
   <si>
@@ -585,6 +577,14 @@
   <si>
     <t>10 (262)
 (258-267)</t>
+  </si>
+  <si>
+    <t>10 (322)
+(314-323)</t>
+  </si>
+  <si>
+    <t>10 (324)
+(324-333)</t>
   </si>
 </sst>
 </file>
@@ -1071,7 +1071,7 @@
   <dimension ref="A1:V22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1155,7 +1155,7 @@
         <v>5</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>6</v>
@@ -1204,59 +1204,59 @@
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="8" t="s">
+      <c r="B3" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="F3" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="G3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="H3" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>26</v>
-      </c>
       <c r="I3" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L3" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="N3" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="O3" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="P3" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="Q3" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="R3" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="S3" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.3">
@@ -1321,58 +1321,58 @@
         <v>3</v>
       </c>
       <c r="B6" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="J6" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="K6" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="L6" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="M6" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="N6" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="C6" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="F6" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="G6" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="H6" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="I6" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="J6" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="K6" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="L6" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="M6" s="8" t="s">
+      <c r="O6" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="N6" s="8" t="s">
+      <c r="P6" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="O6" s="8" t="s">
+      <c r="Q6" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="P6" s="8" t="s">
+      <c r="R6" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="Q6" s="8" t="s">
+      <c r="S6" s="8" t="s">
         <v>80</v>
-      </c>
-      <c r="R6" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="S6" s="8" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
@@ -1380,58 +1380,58 @@
         <v>2</v>
       </c>
       <c r="B7" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="E7" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="F7" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="G7" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="H7" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="G7" s="14" t="s">
+      <c r="I7" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="H7" s="14" t="s">
+      <c r="J7" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="I7" s="14" t="s">
+      <c r="K7" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="J7" s="14" t="s">
+      <c r="L7" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="K7" s="14" t="s">
+      <c r="M7" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="L7" s="14" t="s">
+      <c r="N7" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="M7" s="14" t="s">
+      <c r="O7" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="N7" s="14" t="s">
+      <c r="P7" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="O7" s="14" t="s">
+      <c r="Q7" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="P7" s="14" t="s">
+      <c r="R7" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="Q7" s="14" t="s">
+      <c r="S7" s="14" t="s">
         <v>43</v>
-      </c>
-      <c r="R7" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="S7" s="14" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.3">
@@ -1496,58 +1496,58 @@
         <v>3</v>
       </c>
       <c r="B10" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="E10" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="F10" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="G10" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="H10" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="G10" s="8" t="s">
+      <c r="I10" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="H10" s="8" t="s">
+      <c r="J10" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="I10" s="8" t="s">
+      <c r="K10" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="J10" s="8" t="s">
+      <c r="L10" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="K10" s="8" t="s">
+      <c r="M10" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="L10" s="8" t="s">
+      <c r="N10" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="M10" s="8" t="s">
+      <c r="O10" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="N10" s="8" t="s">
+      <c r="P10" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="O10" s="8" t="s">
+      <c r="Q10" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="P10" s="8" t="s">
+      <c r="R10" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="Q10" s="8" t="s">
+      <c r="S10" s="8" t="s">
         <v>98</v>
-      </c>
-      <c r="R10" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="S10" s="8" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
@@ -1555,58 +1555,58 @@
         <v>2</v>
       </c>
       <c r="B11" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="E11" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="F11" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="G11" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="F11" s="14" t="s">
+      <c r="H11" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="G11" s="14" t="s">
+      <c r="I11" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="H11" s="14" t="s">
+      <c r="J11" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="I11" s="14" t="s">
+      <c r="K11" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="J11" s="14" t="s">
+      <c r="L11" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="K11" s="14" t="s">
+      <c r="M11" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="L11" s="14" t="s">
+      <c r="N11" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="M11" s="14" t="s">
+      <c r="O11" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="N11" s="14" t="s">
+      <c r="P11" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="O11" s="14" t="s">
+      <c r="Q11" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="P11" s="14" t="s">
+      <c r="R11" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="Q11" s="14" t="s">
+      <c r="S11" s="14" t="s">
         <v>61</v>
-      </c>
-      <c r="R11" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="S11" s="14" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.3">
@@ -1671,58 +1671,58 @@
         <v>3</v>
       </c>
       <c r="B14" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="D14" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="E14" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="F14" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="G14" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="F14" s="8" t="s">
+      <c r="H14" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="G14" s="8" t="s">
+      <c r="I14" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="H14" s="8" t="s">
+      <c r="J14" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="I14" s="8" t="s">
+      <c r="K14" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="J14" s="8" t="s">
+      <c r="L14" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="K14" s="8" t="s">
+      <c r="M14" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="L14" s="8" t="s">
+      <c r="N14" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="M14" s="8" t="s">
+      <c r="O14" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="N14" s="8" t="s">
+      <c r="P14" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="O14" s="8" t="s">
+      <c r="Q14" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="P14" s="8" t="s">
+      <c r="R14" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="Q14" s="8" t="s">
+      <c r="S14" s="8" t="s">
         <v>116</v>
-      </c>
-      <c r="R14" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="S14" s="8" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="15" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
@@ -1730,58 +1730,58 @@
         <v>2</v>
       </c>
       <c r="B15" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="E15" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="F15" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="E15" s="14" t="s">
+      <c r="G15" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="F15" s="14" t="s">
+      <c r="H15" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="G15" s="14" t="s">
+      <c r="I15" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="H15" s="14" t="s">
+      <c r="J15" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="I15" s="14" t="s">
+      <c r="K15" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="J15" s="14" t="s">
+      <c r="L15" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="K15" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="L15" s="14" t="s">
-        <v>74</v>
-      </c>
       <c r="M15" s="13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="N15" s="13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="O15" s="13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="P15" s="13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="Q15" s="13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="R15" s="13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="S15" s="13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.3">
@@ -1846,58 +1846,58 @@
         <v>3</v>
       </c>
       <c r="B18" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="D18" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="E18" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="F18" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="G18" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="F18" s="8" t="s">
+      <c r="H18" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="G18" s="8" t="s">
+      <c r="I18" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="H18" s="8" t="s">
+      <c r="J18" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="I18" s="8" t="s">
+      <c r="K18" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="J18" s="8" t="s">
+      <c r="L18" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="K18" s="8" t="s">
+      <c r="M18" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="L18" s="8" t="s">
+      <c r="N18" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="M18" s="8" t="s">
+      <c r="O18" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="N18" s="8" t="s">
+      <c r="P18" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="O18" s="8" t="s">
+      <c r="Q18" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="P18" s="8" t="s">
+      <c r="R18" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="Q18" s="8" t="s">
+      <c r="S18" s="8" t="s">
         <v>134</v>
-      </c>
-      <c r="R18" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="S18" s="8" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="19" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
@@ -1905,58 +1905,58 @@
         <v>2</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G19" s="13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H19" s="13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I19" s="13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J19" s="13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="K19" s="13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L19" s="13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="M19" s="13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="N19" s="13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="O19" s="13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="P19" s="13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="Q19" s="13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="R19" s="13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="S19" s="13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.3">
@@ -1973,10 +1973,10 @@
         <v>3</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v.2 of my Self Improvement Plan
</commit_message>
<xml_diff>
--- a/PLAN_Workflow.xlsx
+++ b/PLAN_Workflow.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="225">
   <si>
     <t>Book "Refactoring"
 (read)</t>
@@ -367,110 +367,7 @@
     <t>My Web App (base)</t>
   </si>
   <si>
-    <t>GIT (doc)</t>
-  </si>
-  <si>
-    <t>My Web App (advanced and API)</t>
-  </si>
-  <si>
-    <t>My Web App (base) / 
-My Web App (advanced and API)</t>
-  </si>
-  <si>
     <t>finish base features</t>
-  </si>
-  <si>
-    <t>(2.1-2.2)</t>
-  </si>
-  <si>
-    <t>(2.3-2.4)</t>
-  </si>
-  <si>
-    <t>(2.5-2.6)</t>
-  </si>
-  <si>
-    <t>(2.7-2.8)</t>
-  </si>
-  <si>
-    <t>(3.1-3.2)</t>
-  </si>
-  <si>
-    <t>(3.3-3.4)</t>
-  </si>
-  <si>
-    <t>(3.5-3.6)</t>
-  </si>
-  <si>
-    <t>(3.7-4.1)</t>
-  </si>
-  <si>
-    <t>(4.2-4.3)</t>
-  </si>
-  <si>
-    <t>(4.4-4.5)</t>
-  </si>
-  <si>
-    <t>(4.6-4.7)</t>
-  </si>
-  <si>
-    <t>(4.8-4.9)</t>
-  </si>
-  <si>
-    <t>(4.10-5.1)</t>
-  </si>
-  <si>
-    <t>(5.2-5.3)</t>
-  </si>
-  <si>
-    <t>(5.4-6.1)</t>
-  </si>
-  <si>
-    <t>(6.2-6.3)</t>
-  </si>
-  <si>
-    <t>(6.4-6.5)</t>
-  </si>
-  <si>
-    <t>(6.6-7.1)</t>
-  </si>
-  <si>
-    <t>(7.2-7.3)</t>
-  </si>
-  <si>
-    <t>(7.4-7.5)</t>
-  </si>
-  <si>
-    <t>(7.6-7.7)</t>
-  </si>
-  <si>
-    <t>(7.8-7.9)</t>
-  </si>
-  <si>
-    <t>(7.10-7.11)</t>
-  </si>
-  <si>
-    <t>(7.12-7.13)</t>
-  </si>
-  <si>
-    <t>(7.14-7.15)</t>
-  </si>
-  <si>
-    <t>(8.1-8.2)</t>
-  </si>
-  <si>
-    <t>(8.3-8.4)</t>
-  </si>
-  <si>
-    <t>(8.5-9.1)</t>
-  </si>
-  <si>
-    <t>(9.2-9.3)</t>
-  </si>
-  <si>
-    <t>(10.1-10.2)</t>
-  </si>
-  <si>
-    <t>(10.3-10.4)</t>
   </si>
   <si>
     <t>10 (380)
@@ -751,8 +648,239 @@
     <t>project from work</t>
   </si>
   <si>
-    <t>10(788)
+    <t>10(792)
 (785-794)</t>
+  </si>
+  <si>
+    <t>Х</t>
+  </si>
+  <si>
+    <t>My Web App (base) / project from work</t>
+  </si>
+  <si>
+    <t>Project from work</t>
+  </si>
+  <si>
+    <t>Pro C# 7: With .NET and .NET Core 8th ed. Edition</t>
+  </si>
+  <si>
+    <t>Design Patterns Elements of reusable Object-Oriented Software (GoF)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Pro C# 7: With .NET and .NET Core 8th ed. Edition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+(11-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+(1-10)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+(21-30)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+(31-40)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+(41-50)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+(51-60)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+(61-70)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+(71-80)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+(81-90)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+(91-100)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+(101-110)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+(111-120)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+(121-130)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+(131-140)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+(141-150)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+(151-160)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+(161-170)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+(171-180)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+(181-190)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+(191-200)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+(201-210)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+(211-220)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+(221-230)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+(231-240)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+(241-250)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+(251-260)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+(261-270)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+(271-280)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+(281-290)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+(291-300)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+(301-310)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+(311-320)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+(321-330)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+(331-340)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+(341-350)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+(351-360)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+(361-370)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+(371-380)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+(381-390)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+(391-396)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+(391-400)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+(401-410)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+(411-420)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+(421-430)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+(431-440)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+(441-450)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+(451-460)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+(461-470)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+(471-480)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+(481-490)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+(491-500)</t>
+  </si>
+  <si>
+    <t>Project from work / Family Economic my web app (base and advanced)</t>
+  </si>
+  <si>
+    <t>my project</t>
+  </si>
+  <si>
+    <t>Family Economic my web app (base and advanced)</t>
   </si>
 </sst>
 </file>
@@ -827,7 +955,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -889,6 +1017,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -966,7 +1100,7 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="4" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="4" applyFont="1" applyBorder="1"/>
@@ -1026,15 +1160,27 @@
     <xf numFmtId="49" fontId="8" fillId="7" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="16" fontId="8" fillId="11" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="7" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1355,10 +1501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:V29"/>
+  <dimension ref="A2:V46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1475,10 +1621,10 @@
         <v>7</v>
       </c>
       <c r="P3" s="13" t="s">
-        <v>125</v>
+        <v>91</v>
       </c>
       <c r="Q3" s="13" t="s">
-        <v>126</v>
+        <v>92</v>
       </c>
       <c r="R3" s="13" t="s">
         <v>8</v>
@@ -1608,46 +1754,46 @@
         <v>3</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>128</v>
+        <v>94</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>129</v>
+        <v>95</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>134</v>
+        <v>100</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>136</v>
+        <v>102</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>137</v>
+        <v>103</v>
       </c>
       <c r="G9" s="19" t="s">
-        <v>139</v>
+        <v>105</v>
       </c>
       <c r="H9" s="19" t="s">
-        <v>143</v>
+        <v>109</v>
       </c>
       <c r="I9" s="19" t="s">
         <v>25</v>
       </c>
       <c r="J9" s="19" t="s">
-        <v>146</v>
+        <v>112</v>
       </c>
       <c r="K9" s="19" t="s">
-        <v>149</v>
+        <v>115</v>
       </c>
       <c r="L9" s="19" t="s">
-        <v>150</v>
+        <v>116</v>
       </c>
       <c r="M9" s="19" t="s">
-        <v>154</v>
+        <v>120</v>
       </c>
       <c r="N9" s="19" t="s">
-        <v>155</v>
+        <v>121</v>
       </c>
       <c r="O9" s="19" t="s">
-        <v>157</v>
+        <v>123</v>
       </c>
       <c r="P9" s="20" t="s">
         <v>26</v>
@@ -1656,54 +1802,54 @@
       <c r="R9" s="21"/>
       <c r="S9" s="21"/>
     </row>
-    <row r="10" spans="1:22" ht="43.15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
       <c r="B10" s="22" t="s">
-        <v>132</v>
-      </c>
-      <c r="C10" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="C10" s="29" t="s">
         <v>14</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>133</v>
+        <v>99</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>135</v>
+        <v>101</v>
       </c>
       <c r="F10" s="22" t="s">
-        <v>140</v>
+        <v>106</v>
       </c>
       <c r="G10" s="22" t="s">
-        <v>141</v>
+        <v>107</v>
       </c>
       <c r="H10" s="22" t="s">
-        <v>142</v>
+        <v>108</v>
       </c>
       <c r="I10" s="22" t="s">
-        <v>144</v>
+        <v>110</v>
       </c>
       <c r="J10" s="22" t="s">
-        <v>145</v>
+        <v>111</v>
       </c>
       <c r="K10" s="22" t="s">
-        <v>147</v>
+        <v>113</v>
       </c>
       <c r="L10" s="22" t="s">
-        <v>151</v>
+        <v>117</v>
       </c>
       <c r="M10" s="22" t="s">
-        <v>152</v>
+        <v>118</v>
       </c>
       <c r="N10" s="22" t="s">
-        <v>156</v>
+        <v>122</v>
       </c>
       <c r="O10" s="22" t="s">
-        <v>158</v>
+        <v>124</v>
       </c>
       <c r="P10" s="22" t="s">
-        <v>161</v>
+        <v>127</v>
       </c>
       <c r="Q10" s="21"/>
       <c r="R10" s="21"/>
@@ -1720,25 +1866,25 @@
         <v>2</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>127</v>
+        <v>93</v>
       </c>
       <c r="E11" s="22" t="s">
-        <v>130</v>
+        <v>96</v>
       </c>
       <c r="F11" s="22" t="s">
-        <v>131</v>
+        <v>97</v>
       </c>
       <c r="G11" s="22" t="s">
-        <v>138</v>
+        <v>104</v>
       </c>
       <c r="H11" s="22">
         <v>4</v>
       </c>
       <c r="I11" s="22" t="s">
-        <v>148</v>
+        <v>114</v>
       </c>
       <c r="J11" s="22" t="s">
-        <v>148</v>
+        <v>114</v>
       </c>
       <c r="K11" s="22" t="s">
         <v>73</v>
@@ -1747,25 +1893,25 @@
         <v>73</v>
       </c>
       <c r="M11" s="22" t="s">
-        <v>153</v>
+        <v>119</v>
       </c>
       <c r="N11" s="22" t="s">
-        <v>159</v>
+        <v>125</v>
       </c>
       <c r="O11" s="22" t="s">
-        <v>160</v>
+        <v>126</v>
       </c>
       <c r="P11" s="22" t="s">
-        <v>162</v>
+        <v>128</v>
       </c>
       <c r="Q11" s="22" t="s">
-        <v>165</v>
+        <v>131</v>
       </c>
       <c r="R11" s="22" t="s">
-        <v>166</v>
+        <v>132</v>
       </c>
       <c r="S11" s="22" t="s">
-        <v>167</v>
+        <v>133</v>
       </c>
     </row>
     <row r="14" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
@@ -1831,49 +1977,49 @@
       </c>
       <c r="B15" s="24"/>
       <c r="C15" s="13" t="s">
-        <v>163</v>
+        <v>129</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>170</v>
+        <v>136</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>172</v>
+        <v>138</v>
       </c>
       <c r="F15" s="19" t="s">
-        <v>174</v>
+        <v>140</v>
       </c>
       <c r="G15" s="28" t="s">
-        <v>176</v>
+        <v>142</v>
       </c>
       <c r="H15" s="28" t="s">
-        <v>178</v>
+        <v>144</v>
       </c>
       <c r="I15" s="28" t="s">
-        <v>183</v>
+        <v>149</v>
       </c>
       <c r="J15" s="28" t="s">
-        <v>184</v>
+        <v>150</v>
       </c>
       <c r="K15" s="28" t="s">
-        <v>187</v>
+        <v>153</v>
       </c>
       <c r="L15" s="28" t="s">
-        <v>188</v>
+        <v>154</v>
       </c>
       <c r="M15" s="19" t="s">
         <v>27</v>
       </c>
       <c r="N15" s="28" t="s">
-        <v>189</v>
+        <v>155</v>
       </c>
       <c r="O15" s="19" t="s">
         <v>28</v>
       </c>
       <c r="P15" s="28" t="s">
-        <v>191</v>
+        <v>157</v>
       </c>
       <c r="Q15" s="28" t="s">
-        <v>193</v>
+        <v>159</v>
       </c>
       <c r="R15" s="19" t="s">
         <v>29</v>
@@ -1889,28 +2035,28 @@
       <c r="B16" s="21"/>
       <c r="C16" s="21"/>
       <c r="D16" s="22" t="s">
-        <v>164</v>
+        <v>130</v>
       </c>
       <c r="E16" s="22" t="s">
-        <v>171</v>
+        <v>137</v>
       </c>
       <c r="F16" s="22" t="s">
-        <v>175</v>
+        <v>141</v>
       </c>
       <c r="G16" s="29" t="s">
-        <v>177</v>
+        <v>143</v>
       </c>
       <c r="H16" s="29" t="s">
-        <v>182</v>
+        <v>148</v>
       </c>
       <c r="I16" s="29" t="s">
-        <v>181</v>
+        <v>147</v>
       </c>
       <c r="J16" s="29" t="s">
         <v>15</v>
       </c>
       <c r="K16" s="29" t="s">
-        <v>185</v>
+        <v>151</v>
       </c>
       <c r="L16" s="22" t="s">
         <v>16</v>
@@ -1922,78 +2068,78 @@
         <v>18</v>
       </c>
       <c r="O16" s="29" t="s">
-        <v>186</v>
+        <v>152</v>
       </c>
       <c r="P16" s="29" t="s">
-        <v>190</v>
+        <v>156</v>
       </c>
       <c r="Q16" s="22" t="s">
         <v>19</v>
       </c>
       <c r="R16" s="29" t="s">
-        <v>192</v>
+        <v>158</v>
       </c>
       <c r="S16" s="29" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" ht="73.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="14" t="s">
-        <v>89</v>
+        <v>161</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="35" t="s">
+        <v>166</v>
       </c>
       <c r="B17" s="22" t="s">
-        <v>168</v>
+        <v>134</v>
       </c>
       <c r="C17" s="22" t="s">
-        <v>168</v>
+        <v>134</v>
       </c>
       <c r="D17" s="22" t="s">
-        <v>169</v>
+        <v>135</v>
       </c>
       <c r="E17" s="22" t="s">
-        <v>173</v>
+        <v>139</v>
       </c>
       <c r="F17" s="29" t="s">
-        <v>179</v>
+        <v>145</v>
       </c>
       <c r="G17" s="29" t="s">
-        <v>180</v>
+        <v>146</v>
       </c>
       <c r="H17" s="29" t="s">
-        <v>197</v>
+        <v>163</v>
       </c>
       <c r="I17" s="22" t="s">
-        <v>197</v>
+        <v>163</v>
       </c>
       <c r="J17" s="22" t="s">
-        <v>197</v>
+        <v>163</v>
       </c>
       <c r="K17" s="22" t="s">
-        <v>197</v>
+        <v>163</v>
       </c>
       <c r="L17" s="22" t="s">
-        <v>197</v>
+        <v>163</v>
       </c>
       <c r="M17" s="22" t="s">
-        <v>197</v>
+        <v>163</v>
       </c>
       <c r="N17" s="22" t="s">
-        <v>197</v>
+        <v>163</v>
       </c>
       <c r="O17" s="22" t="s">
-        <v>197</v>
+        <v>163</v>
       </c>
       <c r="P17" s="22" t="s">
-        <v>197</v>
+        <v>163</v>
       </c>
       <c r="Q17" s="22" t="s">
-        <v>197</v>
+        <v>163</v>
       </c>
       <c r="R17" s="22" t="s">
-        <v>197</v>
+        <v>163</v>
       </c>
       <c r="S17" s="22" t="s">
-        <v>197</v>
+        <v>163</v>
       </c>
     </row>
     <row r="20" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
@@ -2028,10 +2174,10 @@
       <c r="K20" s="18">
         <v>43083</v>
       </c>
-      <c r="L20" s="32">
+      <c r="L20" s="18">
         <v>43084</v>
       </c>
-      <c r="M20" s="23">
+      <c r="M20" s="31">
         <v>43087</v>
       </c>
       <c r="N20" s="23">
@@ -2058,10 +2204,10 @@
         <v>3</v>
       </c>
       <c r="B21" s="28" t="s">
-        <v>194</v>
+        <v>160</v>
       </c>
       <c r="C21" s="28" t="s">
-        <v>196</v>
+        <v>162</v>
       </c>
       <c r="D21" s="19" t="s">
         <v>31</v>
@@ -2084,13 +2230,13 @@
       <c r="J21" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="K21" s="33" t="s">
-        <v>198</v>
+      <c r="K21" s="32" t="s">
+        <v>164</v>
       </c>
       <c r="L21" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="M21" s="25" t="s">
+      <c r="M21" s="30" t="s">
         <v>39</v>
       </c>
       <c r="N21" s="25" t="s">
@@ -2112,9 +2258,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" ht="48.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
-        <v>90</v>
+        <v>2</v>
       </c>
       <c r="B22" s="22" t="s">
         <v>20</v>
@@ -2131,103 +2277,103 @@
       <c r="F22" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="G22" s="31" t="s">
-        <v>94</v>
-      </c>
-      <c r="H22" s="26" t="s">
-        <v>95</v>
-      </c>
-      <c r="I22" s="26" t="s">
-        <v>96</v>
-      </c>
-      <c r="J22" s="26" t="s">
-        <v>97</v>
-      </c>
-      <c r="K22" s="26" t="s">
-        <v>98</v>
-      </c>
-      <c r="L22" s="26" t="s">
-        <v>99</v>
-      </c>
-      <c r="M22" s="26" t="s">
-        <v>100</v>
-      </c>
-      <c r="N22" s="26" t="s">
-        <v>101</v>
-      </c>
-      <c r="O22" s="26" t="s">
-        <v>102</v>
-      </c>
-      <c r="P22" s="26" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q22" s="26" t="s">
-        <v>104</v>
-      </c>
-      <c r="R22" s="26" t="s">
-        <v>105</v>
-      </c>
-      <c r="S22" s="26" t="s">
-        <v>106</v>
+      <c r="G22" s="34" t="s">
+        <v>165</v>
+      </c>
+      <c r="H22" s="34" t="s">
+        <v>165</v>
+      </c>
+      <c r="I22" s="34" t="s">
+        <v>165</v>
+      </c>
+      <c r="J22" s="34" t="s">
+        <v>165</v>
+      </c>
+      <c r="K22" s="34" t="s">
+        <v>165</v>
+      </c>
+      <c r="L22" s="34" t="s">
+        <v>165</v>
+      </c>
+      <c r="M22" s="34" t="s">
+        <v>165</v>
+      </c>
+      <c r="N22" s="34" t="s">
+        <v>165</v>
+      </c>
+      <c r="O22" s="34" t="s">
+        <v>165</v>
+      </c>
+      <c r="P22" s="34" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q22" s="34" t="s">
+        <v>165</v>
+      </c>
+      <c r="R22" s="34" t="s">
+        <v>165</v>
+      </c>
+      <c r="S22" s="34" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="23" spans="1:19" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="14" t="s">
-        <v>92</v>
+      <c r="A23" s="35" t="s">
+        <v>167</v>
       </c>
       <c r="B23" s="22" t="s">
-        <v>197</v>
+        <v>163</v>
       </c>
       <c r="C23" s="22" t="s">
-        <v>197</v>
+        <v>163</v>
       </c>
       <c r="D23" s="22" t="s">
-        <v>197</v>
+        <v>163</v>
       </c>
       <c r="E23" s="22" t="s">
-        <v>197</v>
+        <v>163</v>
       </c>
       <c r="F23" s="22" t="s">
-        <v>197</v>
+        <v>163</v>
       </c>
       <c r="G23" s="22" t="s">
-        <v>197</v>
-      </c>
-      <c r="H23" s="34" t="s">
-        <v>93</v>
+        <v>163</v>
+      </c>
+      <c r="H23" s="33" t="s">
+        <v>90</v>
       </c>
       <c r="I23" s="22" t="s">
-        <v>197</v>
+        <v>163</v>
       </c>
       <c r="J23" s="22" t="s">
-        <v>197</v>
-      </c>
-      <c r="K23" s="22" t="s">
-        <v>197</v>
+        <v>163</v>
+      </c>
+      <c r="K23" s="29" t="s">
+        <v>163</v>
       </c>
       <c r="L23" s="22" t="s">
-        <v>197</v>
-      </c>
-      <c r="M23" s="26" t="s">
-        <v>197</v>
+        <v>163</v>
+      </c>
+      <c r="M23" s="22" t="s">
+        <v>163</v>
       </c>
       <c r="N23" s="26" t="s">
-        <v>197</v>
+        <v>163</v>
       </c>
       <c r="O23" s="26" t="s">
-        <v>197</v>
+        <v>163</v>
       </c>
       <c r="P23" s="26" t="s">
-        <v>197</v>
+        <v>163</v>
       </c>
       <c r="Q23" s="26" t="s">
-        <v>197</v>
+        <v>163</v>
       </c>
       <c r="R23" s="26" t="s">
-        <v>197</v>
+        <v>163</v>
       </c>
       <c r="S23" s="26" t="s">
-        <v>197</v>
+        <v>163</v>
       </c>
     </row>
     <row r="24" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
@@ -2290,7 +2436,7 @@
         <v>43122</v>
       </c>
     </row>
-    <row r="27" spans="1:19" ht="43.15" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
         <v>3</v>
       </c>
@@ -2333,93 +2479,821 @@
       <c r="N27" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="O27" s="26"/>
-      <c r="P27" s="26"/>
-      <c r="Q27" s="26"/>
-      <c r="R27" s="26"/>
-      <c r="S27" s="26"/>
-    </row>
-    <row r="28" spans="1:19" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="B28" s="26" t="s">
-        <v>107</v>
-      </c>
-      <c r="C28" s="26" t="s">
-        <v>108</v>
-      </c>
-      <c r="D28" s="26" t="s">
-        <v>109</v>
-      </c>
-      <c r="E28" s="26" t="s">
-        <v>110</v>
-      </c>
-      <c r="F28" s="26" t="s">
-        <v>111</v>
-      </c>
-      <c r="G28" s="26" t="s">
-        <v>112</v>
-      </c>
-      <c r="H28" s="26" t="s">
-        <v>113</v>
-      </c>
-      <c r="I28" s="26" t="s">
-        <v>114</v>
-      </c>
-      <c r="J28" s="26" t="s">
-        <v>115</v>
-      </c>
-      <c r="K28" s="26" t="s">
-        <v>116</v>
-      </c>
-      <c r="L28" s="26" t="s">
-        <v>117</v>
-      </c>
-      <c r="M28" s="26" t="s">
-        <v>118</v>
-      </c>
-      <c r="N28" s="26" t="s">
-        <v>119</v>
-      </c>
-      <c r="O28" s="26" t="s">
-        <v>120</v>
-      </c>
-      <c r="P28" s="26" t="s">
-        <v>121</v>
-      </c>
-      <c r="Q28" s="26" t="s">
-        <v>122</v>
-      </c>
-      <c r="R28" s="26" t="s">
-        <v>123</v>
-      </c>
-      <c r="S28" s="26" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19" ht="42" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="B29" s="26"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="26"/>
-      <c r="K29" s="26"/>
-      <c r="L29" s="26"/>
-      <c r="M29" s="26"/>
-      <c r="N29" s="26"/>
-      <c r="O29" s="26"/>
-      <c r="P29" s="26"/>
-      <c r="Q29" s="26"/>
-      <c r="R29" s="26"/>
-      <c r="S29" s="26"/>
+      <c r="O27" s="37" t="s">
+        <v>172</v>
+      </c>
+      <c r="P27" s="37" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q27" s="37" t="s">
+        <v>173</v>
+      </c>
+      <c r="R27" s="37" t="s">
+        <v>174</v>
+      </c>
+      <c r="S27" s="37" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" ht="81" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="35" t="s">
+        <v>169</v>
+      </c>
+      <c r="B28" s="34" t="s">
+        <v>165</v>
+      </c>
+      <c r="C28" s="34" t="s">
+        <v>165</v>
+      </c>
+      <c r="D28" s="34" t="s">
+        <v>165</v>
+      </c>
+      <c r="E28" s="34" t="s">
+        <v>165</v>
+      </c>
+      <c r="F28" s="34" t="s">
+        <v>165</v>
+      </c>
+      <c r="G28" s="34" t="s">
+        <v>165</v>
+      </c>
+      <c r="H28" s="34" t="s">
+        <v>165</v>
+      </c>
+      <c r="I28" s="34" t="s">
+        <v>165</v>
+      </c>
+      <c r="J28" s="34" t="s">
+        <v>165</v>
+      </c>
+      <c r="K28" s="34" t="s">
+        <v>165</v>
+      </c>
+      <c r="L28" s="34" t="s">
+        <v>165</v>
+      </c>
+      <c r="M28" s="34" t="s">
+        <v>165</v>
+      </c>
+      <c r="N28" s="34" t="s">
+        <v>165</v>
+      </c>
+      <c r="O28" s="37" t="s">
+        <v>172</v>
+      </c>
+      <c r="P28" s="37" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q28" s="37" t="s">
+        <v>173</v>
+      </c>
+      <c r="R28" s="37" t="s">
+        <v>174</v>
+      </c>
+      <c r="S28" s="37" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="35" t="s">
+        <v>167</v>
+      </c>
+      <c r="B29" s="38" t="s">
+        <v>163</v>
+      </c>
+      <c r="C29" s="38" t="s">
+        <v>163</v>
+      </c>
+      <c r="D29" s="38" t="s">
+        <v>163</v>
+      </c>
+      <c r="E29" s="38" t="s">
+        <v>163</v>
+      </c>
+      <c r="F29" s="38" t="s">
+        <v>163</v>
+      </c>
+      <c r="G29" s="38" t="s">
+        <v>163</v>
+      </c>
+      <c r="H29" s="38" t="s">
+        <v>163</v>
+      </c>
+      <c r="I29" s="38" t="s">
+        <v>163</v>
+      </c>
+      <c r="J29" s="38" t="s">
+        <v>163</v>
+      </c>
+      <c r="K29" s="38" t="s">
+        <v>163</v>
+      </c>
+      <c r="L29" s="38" t="s">
+        <v>163</v>
+      </c>
+      <c r="M29" s="38" t="s">
+        <v>163</v>
+      </c>
+      <c r="N29" s="38" t="s">
+        <v>163</v>
+      </c>
+      <c r="O29" s="38" t="s">
+        <v>163</v>
+      </c>
+      <c r="P29" s="38" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q29" s="38" t="s">
+        <v>163</v>
+      </c>
+      <c r="R29" s="38" t="s">
+        <v>163</v>
+      </c>
+      <c r="S29" s="38" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A31" s="17"/>
+      <c r="B31" s="23">
+        <v>43123</v>
+      </c>
+      <c r="C31" s="23">
+        <v>43124</v>
+      </c>
+      <c r="D31" s="23">
+        <v>43125</v>
+      </c>
+      <c r="E31" s="23">
+        <v>43126</v>
+      </c>
+      <c r="F31" s="23">
+        <v>43129</v>
+      </c>
+      <c r="G31" s="23">
+        <v>43130</v>
+      </c>
+      <c r="H31" s="23">
+        <v>43131</v>
+      </c>
+      <c r="I31" s="23">
+        <v>43132</v>
+      </c>
+      <c r="J31" s="23">
+        <v>43133</v>
+      </c>
+      <c r="K31" s="23">
+        <v>43136</v>
+      </c>
+      <c r="L31" s="23">
+        <v>43137</v>
+      </c>
+      <c r="M31" s="23">
+        <v>43138</v>
+      </c>
+      <c r="N31" s="23">
+        <v>43139</v>
+      </c>
+      <c r="O31" s="23">
+        <v>43140</v>
+      </c>
+      <c r="P31" s="23">
+        <v>43143</v>
+      </c>
+      <c r="Q31" s="23">
+        <v>43144</v>
+      </c>
+      <c r="R31" s="23">
+        <v>43145</v>
+      </c>
+      <c r="S31" s="23">
+        <v>43146</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="35" t="s">
+        <v>170</v>
+      </c>
+      <c r="B32" s="37" t="s">
+        <v>176</v>
+      </c>
+      <c r="C32" s="37" t="s">
+        <v>177</v>
+      </c>
+      <c r="D32" s="37" t="s">
+        <v>178</v>
+      </c>
+      <c r="E32" s="37" t="s">
+        <v>179</v>
+      </c>
+      <c r="F32" s="37" t="s">
+        <v>180</v>
+      </c>
+      <c r="G32" s="37" t="s">
+        <v>181</v>
+      </c>
+      <c r="H32" s="37" t="s">
+        <v>182</v>
+      </c>
+      <c r="I32" s="37" t="s">
+        <v>183</v>
+      </c>
+      <c r="J32" s="37" t="s">
+        <v>184</v>
+      </c>
+      <c r="K32" s="37" t="s">
+        <v>176</v>
+      </c>
+      <c r="L32" s="37" t="s">
+        <v>177</v>
+      </c>
+      <c r="M32" s="37" t="s">
+        <v>178</v>
+      </c>
+      <c r="N32" s="37" t="s">
+        <v>179</v>
+      </c>
+      <c r="O32" s="37" t="s">
+        <v>180</v>
+      </c>
+      <c r="P32" s="37" t="s">
+        <v>181</v>
+      </c>
+      <c r="Q32" s="37" t="s">
+        <v>182</v>
+      </c>
+      <c r="R32" s="37" t="s">
+        <v>183</v>
+      </c>
+      <c r="S32" s="37" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="35" t="s">
+        <v>169</v>
+      </c>
+      <c r="B33" s="37" t="s">
+        <v>176</v>
+      </c>
+      <c r="C33" s="37" t="s">
+        <v>177</v>
+      </c>
+      <c r="D33" s="37" t="s">
+        <v>178</v>
+      </c>
+      <c r="E33" s="37" t="s">
+        <v>179</v>
+      </c>
+      <c r="F33" s="37" t="s">
+        <v>180</v>
+      </c>
+      <c r="G33" s="37" t="s">
+        <v>181</v>
+      </c>
+      <c r="H33" s="37" t="s">
+        <v>182</v>
+      </c>
+      <c r="I33" s="37" t="s">
+        <v>183</v>
+      </c>
+      <c r="J33" s="37" t="s">
+        <v>184</v>
+      </c>
+      <c r="K33" s="37" t="s">
+        <v>176</v>
+      </c>
+      <c r="L33" s="37" t="s">
+        <v>177</v>
+      </c>
+      <c r="M33" s="37" t="s">
+        <v>178</v>
+      </c>
+      <c r="N33" s="37" t="s">
+        <v>179</v>
+      </c>
+      <c r="O33" s="37" t="s">
+        <v>180</v>
+      </c>
+      <c r="P33" s="37" t="s">
+        <v>181</v>
+      </c>
+      <c r="Q33" s="37" t="s">
+        <v>182</v>
+      </c>
+      <c r="R33" s="37" t="s">
+        <v>183</v>
+      </c>
+      <c r="S33" s="37" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="35" t="s">
+        <v>222</v>
+      </c>
+      <c r="B34" s="38" t="s">
+        <v>163</v>
+      </c>
+      <c r="C34" s="38" t="s">
+        <v>163</v>
+      </c>
+      <c r="D34" s="38" t="s">
+        <v>163</v>
+      </c>
+      <c r="E34" s="38" t="s">
+        <v>163</v>
+      </c>
+      <c r="F34" s="38" t="s">
+        <v>163</v>
+      </c>
+      <c r="G34" s="38" t="s">
+        <v>163</v>
+      </c>
+      <c r="H34" s="38" t="s">
+        <v>163</v>
+      </c>
+      <c r="I34" s="36" t="s">
+        <v>223</v>
+      </c>
+      <c r="J34" s="36" t="s">
+        <v>223</v>
+      </c>
+      <c r="K34" s="36" t="s">
+        <v>223</v>
+      </c>
+      <c r="L34" s="36" t="s">
+        <v>223</v>
+      </c>
+      <c r="M34" s="36" t="s">
+        <v>223</v>
+      </c>
+      <c r="N34" s="36" t="s">
+        <v>223</v>
+      </c>
+      <c r="O34" s="36" t="s">
+        <v>223</v>
+      </c>
+      <c r="P34" s="36" t="s">
+        <v>223</v>
+      </c>
+      <c r="Q34" s="36" t="s">
+        <v>223</v>
+      </c>
+      <c r="R34" s="36" t="s">
+        <v>223</v>
+      </c>
+      <c r="S34" s="36" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A37" s="17"/>
+      <c r="B37" s="23">
+        <v>43146</v>
+      </c>
+      <c r="C37" s="23">
+        <v>43147</v>
+      </c>
+      <c r="D37" s="23">
+        <v>43150</v>
+      </c>
+      <c r="E37" s="23">
+        <v>43151</v>
+      </c>
+      <c r="F37" s="23">
+        <v>43152</v>
+      </c>
+      <c r="G37" s="23">
+        <v>43153</v>
+      </c>
+      <c r="H37" s="23">
+        <v>43154</v>
+      </c>
+      <c r="I37" s="23">
+        <v>43157</v>
+      </c>
+      <c r="J37" s="23">
+        <v>43158</v>
+      </c>
+      <c r="K37" s="23">
+        <v>43159</v>
+      </c>
+      <c r="L37" s="23">
+        <v>43160</v>
+      </c>
+      <c r="M37" s="23">
+        <v>43161</v>
+      </c>
+      <c r="N37" s="23">
+        <v>43164</v>
+      </c>
+      <c r="O37" s="23">
+        <v>43165</v>
+      </c>
+      <c r="P37" s="23">
+        <v>43166</v>
+      </c>
+      <c r="Q37" s="23">
+        <v>43167</v>
+      </c>
+      <c r="R37" s="23">
+        <v>43168</v>
+      </c>
+      <c r="S37" s="23">
+        <v>43171</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+      <c r="A38" s="35" t="s">
+        <v>168</v>
+      </c>
+      <c r="B38" s="37" t="s">
+        <v>185</v>
+      </c>
+      <c r="C38" s="37" t="s">
+        <v>186</v>
+      </c>
+      <c r="D38" s="37" t="s">
+        <v>187</v>
+      </c>
+      <c r="E38" s="37" t="s">
+        <v>188</v>
+      </c>
+      <c r="F38" s="37" t="s">
+        <v>189</v>
+      </c>
+      <c r="G38" s="37" t="s">
+        <v>190</v>
+      </c>
+      <c r="H38" s="37" t="s">
+        <v>191</v>
+      </c>
+      <c r="I38" s="37" t="s">
+        <v>192</v>
+      </c>
+      <c r="J38" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="K38" s="37" t="s">
+        <v>194</v>
+      </c>
+      <c r="L38" s="37" t="s">
+        <v>195</v>
+      </c>
+      <c r="M38" s="37" t="s">
+        <v>196</v>
+      </c>
+      <c r="N38" s="37" t="s">
+        <v>197</v>
+      </c>
+      <c r="O38" s="37" t="s">
+        <v>198</v>
+      </c>
+      <c r="P38" s="37" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q38" s="37" t="s">
+        <v>200</v>
+      </c>
+      <c r="R38" s="37" t="s">
+        <v>201</v>
+      </c>
+      <c r="S38" s="37" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="35" t="s">
+        <v>169</v>
+      </c>
+      <c r="B39" s="37" t="s">
+        <v>185</v>
+      </c>
+      <c r="C39" s="37" t="s">
+        <v>186</v>
+      </c>
+      <c r="D39" s="37" t="s">
+        <v>187</v>
+      </c>
+      <c r="E39" s="37" t="s">
+        <v>188</v>
+      </c>
+      <c r="F39" s="37" t="s">
+        <v>189</v>
+      </c>
+      <c r="G39" s="37" t="s">
+        <v>190</v>
+      </c>
+      <c r="H39" s="37" t="s">
+        <v>191</v>
+      </c>
+      <c r="I39" s="37" t="s">
+        <v>192</v>
+      </c>
+      <c r="J39" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="K39" s="37" t="s">
+        <v>194</v>
+      </c>
+      <c r="L39" s="37" t="s">
+        <v>195</v>
+      </c>
+      <c r="M39" s="37" t="s">
+        <v>196</v>
+      </c>
+      <c r="N39" s="37" t="s">
+        <v>197</v>
+      </c>
+      <c r="O39" s="37" t="s">
+        <v>198</v>
+      </c>
+      <c r="P39" s="37" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q39" s="37" t="s">
+        <v>200</v>
+      </c>
+      <c r="R39" s="37" t="s">
+        <v>201</v>
+      </c>
+      <c r="S39" s="37" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="35" t="s">
+        <v>224</v>
+      </c>
+      <c r="B40" s="36" t="s">
+        <v>223</v>
+      </c>
+      <c r="C40" s="36" t="s">
+        <v>223</v>
+      </c>
+      <c r="D40" s="36" t="s">
+        <v>223</v>
+      </c>
+      <c r="E40" s="36" t="s">
+        <v>223</v>
+      </c>
+      <c r="F40" s="36" t="s">
+        <v>223</v>
+      </c>
+      <c r="G40" s="36" t="s">
+        <v>223</v>
+      </c>
+      <c r="H40" s="36" t="s">
+        <v>223</v>
+      </c>
+      <c r="I40" s="36" t="s">
+        <v>223</v>
+      </c>
+      <c r="J40" s="36" t="s">
+        <v>223</v>
+      </c>
+      <c r="K40" s="36" t="s">
+        <v>223</v>
+      </c>
+      <c r="L40" s="36" t="s">
+        <v>223</v>
+      </c>
+      <c r="M40" s="36" t="s">
+        <v>223</v>
+      </c>
+      <c r="N40" s="36" t="s">
+        <v>223</v>
+      </c>
+      <c r="O40" s="36" t="s">
+        <v>223</v>
+      </c>
+      <c r="P40" s="36" t="s">
+        <v>223</v>
+      </c>
+      <c r="Q40" s="36" t="s">
+        <v>223</v>
+      </c>
+      <c r="R40" s="36" t="s">
+        <v>223</v>
+      </c>
+      <c r="S40" s="36" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A43" s="17"/>
+      <c r="B43" s="23">
+        <v>43172</v>
+      </c>
+      <c r="C43" s="23">
+        <v>43173</v>
+      </c>
+      <c r="D43" s="23">
+        <v>43174</v>
+      </c>
+      <c r="E43" s="23">
+        <v>43175</v>
+      </c>
+      <c r="F43" s="23">
+        <v>43178</v>
+      </c>
+      <c r="G43" s="23">
+        <v>43179</v>
+      </c>
+      <c r="H43" s="23">
+        <v>43180</v>
+      </c>
+      <c r="I43" s="23">
+        <v>43181</v>
+      </c>
+      <c r="J43" s="23">
+        <v>43182</v>
+      </c>
+      <c r="K43" s="23">
+        <v>43185</v>
+      </c>
+      <c r="L43" s="23">
+        <v>43186</v>
+      </c>
+      <c r="M43" s="23">
+        <v>43187</v>
+      </c>
+      <c r="N43" s="23">
+        <v>43188</v>
+      </c>
+      <c r="O43" s="23">
+        <v>43189</v>
+      </c>
+      <c r="P43" s="23">
+        <v>43166</v>
+      </c>
+      <c r="Q43" s="23">
+        <v>43167</v>
+      </c>
+      <c r="R43" s="23">
+        <v>43168</v>
+      </c>
+      <c r="S43" s="23">
+        <v>43171</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+      <c r="A44" s="35" t="s">
+        <v>168</v>
+      </c>
+      <c r="B44" s="37" t="s">
+        <v>203</v>
+      </c>
+      <c r="C44" s="37" t="s">
+        <v>204</v>
+      </c>
+      <c r="D44" s="37" t="s">
+        <v>205</v>
+      </c>
+      <c r="E44" s="37" t="s">
+        <v>206</v>
+      </c>
+      <c r="F44" s="37" t="s">
+        <v>207</v>
+      </c>
+      <c r="G44" s="37" t="s">
+        <v>208</v>
+      </c>
+      <c r="H44" s="37" t="s">
+        <v>209</v>
+      </c>
+      <c r="I44" s="37" t="s">
+        <v>211</v>
+      </c>
+      <c r="J44" s="37" t="s">
+        <v>212</v>
+      </c>
+      <c r="K44" s="37" t="s">
+        <v>213</v>
+      </c>
+      <c r="L44" s="37" t="s">
+        <v>214</v>
+      </c>
+      <c r="M44" s="37" t="s">
+        <v>215</v>
+      </c>
+      <c r="N44" s="37" t="s">
+        <v>216</v>
+      </c>
+      <c r="O44" s="37" t="s">
+        <v>217</v>
+      </c>
+      <c r="P44" s="37" t="s">
+        <v>218</v>
+      </c>
+      <c r="Q44" s="37" t="s">
+        <v>219</v>
+      </c>
+      <c r="R44" s="37" t="s">
+        <v>220</v>
+      </c>
+      <c r="S44" s="37" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" ht="75" x14ac:dyDescent="0.25">
+      <c r="A45" s="35" t="s">
+        <v>169</v>
+      </c>
+      <c r="B45" s="37" t="s">
+        <v>203</v>
+      </c>
+      <c r="C45" s="37" t="s">
+        <v>204</v>
+      </c>
+      <c r="D45" s="37" t="s">
+        <v>205</v>
+      </c>
+      <c r="E45" s="37" t="s">
+        <v>206</v>
+      </c>
+      <c r="F45" s="37" t="s">
+        <v>207</v>
+      </c>
+      <c r="G45" s="37" t="s">
+        <v>208</v>
+      </c>
+      <c r="H45" s="37" t="s">
+        <v>209</v>
+      </c>
+      <c r="I45" s="37" t="s">
+        <v>210</v>
+      </c>
+      <c r="J45" s="26"/>
+      <c r="K45" s="26"/>
+      <c r="L45" s="26"/>
+      <c r="M45" s="26"/>
+      <c r="N45" s="26"/>
+      <c r="O45" s="26"/>
+      <c r="P45" s="26"/>
+      <c r="Q45" s="26"/>
+      <c r="R45" s="26"/>
+      <c r="S45" s="26"/>
+    </row>
+    <row r="46" spans="1:19" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="35" t="s">
+        <v>224</v>
+      </c>
+      <c r="B46" s="36" t="s">
+        <v>223</v>
+      </c>
+      <c r="C46" s="36" t="s">
+        <v>223</v>
+      </c>
+      <c r="D46" s="36" t="s">
+        <v>223</v>
+      </c>
+      <c r="E46" s="36" t="s">
+        <v>223</v>
+      </c>
+      <c r="F46" s="36" t="s">
+        <v>223</v>
+      </c>
+      <c r="G46" s="36" t="s">
+        <v>223</v>
+      </c>
+      <c r="H46" s="36" t="s">
+        <v>223</v>
+      </c>
+      <c r="I46" s="36" t="s">
+        <v>223</v>
+      </c>
+      <c r="J46" s="36" t="s">
+        <v>223</v>
+      </c>
+      <c r="K46" s="36" t="s">
+        <v>223</v>
+      </c>
+      <c r="L46" s="36" t="s">
+        <v>223</v>
+      </c>
+      <c r="M46" s="36" t="s">
+        <v>223</v>
+      </c>
+      <c r="N46" s="36" t="s">
+        <v>223</v>
+      </c>
+      <c r="O46" s="36" t="s">
+        <v>223</v>
+      </c>
+      <c r="P46" s="36" t="s">
+        <v>223</v>
+      </c>
+      <c r="Q46" s="36" t="s">
+        <v>223</v>
+      </c>
+      <c r="R46" s="36" t="s">
+        <v>223</v>
+      </c>
+      <c r="S46" s="36" t="s">
+        <v>223</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
.net, DP, and DP rescheduled
</commit_message>
<xml_diff>
--- a/PLAN_Workflow.xlsx
+++ b/PLAN_Workflow.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="290">
   <si>
     <t>Book "Refactoring"
 (read)</t>
@@ -639,14 +639,6 @@
   </si>
   <si>
     <t xml:space="preserve">
-(51-60)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-(61-70)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
 (71-80)</t>
   </si>
   <si>
@@ -895,8 +887,219 @@
 (51-60)</t>
   </si>
   <si>
+    <t>64
+(61-70)</t>
+  </si>
+  <si>
     <t>51
-(51-60)</t>
+(51-55)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+(61-65)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+(66-70)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+(71-75)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+(76-80)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+(81-85)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+(86-90)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+(91-95)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+(96-100)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+(101-105)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+(106-110)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+(111-115)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+(116-120)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+(121-125)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+(126-130)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+(131-135)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+(136-140)</t>
+  </si>
+  <si>
+    <t>(501-510)</t>
+  </si>
+  <si>
+    <t>(511-520)</t>
+  </si>
+  <si>
+    <t>(521-530)</t>
+  </si>
+  <si>
+    <t>(531-540)</t>
+  </si>
+  <si>
+    <t>(541-550)</t>
+  </si>
+  <si>
+    <t>(551-560)</t>
+  </si>
+  <si>
+    <t>(561-570)</t>
+  </si>
+  <si>
+    <t>(571-580)</t>
+  </si>
+  <si>
+    <t>(581-590)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+(141-145)</t>
+  </si>
+  <si>
+    <t>(146-150)</t>
+  </si>
+  <si>
+    <t>(151-155)</t>
+  </si>
+  <si>
+    <t>(156-160)</t>
+  </si>
+  <si>
+    <t>(161-165)</t>
+  </si>
+  <si>
+    <t>(166-170)</t>
+  </si>
+  <si>
+    <t>(171-175)</t>
+  </si>
+  <si>
+    <t>(176-180)</t>
+  </si>
+  <si>
+    <t>(181-185)</t>
+  </si>
+  <si>
+    <t>(186-190)</t>
+  </si>
+  <si>
+    <t>(191-195)</t>
+  </si>
+  <si>
+    <t>(196-200)</t>
+  </si>
+  <si>
+    <t>(201-205)</t>
+  </si>
+  <si>
+    <t>(206-210)</t>
+  </si>
+  <si>
+    <t>(211-215)</t>
+  </si>
+  <si>
+    <t>(216-220)</t>
+  </si>
+  <si>
+    <t>(221-225)</t>
+  </si>
+  <si>
+    <t>(226-230)</t>
+  </si>
+  <si>
+    <t>(231-235)</t>
+  </si>
+  <si>
+    <t>(236-240)</t>
+  </si>
+  <si>
+    <t>(241-245)</t>
+  </si>
+  <si>
+    <t>(246-250)</t>
+  </si>
+  <si>
+    <t>(251-255)</t>
+  </si>
+  <si>
+    <t>(256-260)</t>
+  </si>
+  <si>
+    <t>(261-265)</t>
+  </si>
+  <si>
+    <t>(266-270)</t>
+  </si>
+  <si>
+    <t>(271-275)</t>
+  </si>
+  <si>
+    <t>(276-280)</t>
+  </si>
+  <si>
+    <t>(281-285)</t>
+  </si>
+  <si>
+    <t>(286-290)</t>
+  </si>
+  <si>
+    <t>(291-295)</t>
+  </si>
+  <si>
+    <t>(296-300)</t>
+  </si>
+  <si>
+    <t>(301-305)</t>
+  </si>
+  <si>
+    <t>(306-310)</t>
+  </si>
+  <si>
+    <t>(311-315)</t>
+  </si>
+  <si>
+    <t>(316-320)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> latest pages of GoF</t>
+  </si>
+  <si>
+    <t>56
+(56-60)</t>
   </si>
 </sst>
 </file>
@@ -977,7 +1180,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1045,12 +1248,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1198,9 +1395,7 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="20% - Акцент1" xfId="2" builtinId="30"/>
@@ -1520,10 +1715,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:V42"/>
+  <dimension ref="A2:V46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U42" sqref="U42"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2256,22 +2451,22 @@
         <v>38</v>
       </c>
       <c r="M20" s="26" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="N20" s="26" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="O20" s="19" t="s">
         <v>39</v>
       </c>
       <c r="P20" s="26" t="s">
+        <v>209</v>
+      </c>
+      <c r="Q20" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="R20" s="26" t="s">
         <v>211</v>
-      </c>
-      <c r="Q20" s="26" t="s">
-        <v>212</v>
-      </c>
-      <c r="R20" s="26" t="s">
-        <v>213</v>
       </c>
       <c r="S20" s="19" t="s">
         <v>40</v>
@@ -2457,25 +2652,25 @@
     </row>
     <row r="26" spans="1:19" ht="90" x14ac:dyDescent="0.25">
       <c r="A26" s="31" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B26" s="26" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C26" s="19" t="s">
         <v>41</v>
       </c>
       <c r="D26" s="26" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E26" s="26" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F26" s="19" t="s">
         <v>42</v>
       </c>
       <c r="G26" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="H26" s="19" t="s">
         <v>43</v>
@@ -2487,16 +2682,16 @@
         <v>45</v>
       </c>
       <c r="K26" s="33" t="s">
+        <v>216</v>
+      </c>
+      <c r="L26" s="26" t="s">
+        <v>217</v>
+      </c>
+      <c r="M26" s="26" t="s">
         <v>218</v>
       </c>
-      <c r="L26" s="26" t="s">
-        <v>219</v>
-      </c>
-      <c r="M26" s="26" t="s">
+      <c r="N26" s="26" t="s">
         <v>220</v>
-      </c>
-      <c r="N26" s="26" t="s">
-        <v>222</v>
       </c>
       <c r="O26" s="27" t="s">
         <v>159</v>
@@ -2511,7 +2706,7 @@
         <v>161</v>
       </c>
       <c r="S26" s="27" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="27" spans="1:19" ht="81" customHeight="1" x14ac:dyDescent="0.25">
@@ -2558,13 +2753,13 @@
         <v>152</v>
       </c>
       <c r="O27" s="27" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="P27" s="27" t="s">
         <v>158</v>
       </c>
       <c r="Q27" s="27" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="R27" s="27" t="s">
         <v>161</v>
@@ -2575,10 +2770,10 @@
     </row>
     <row r="30" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A30" s="17"/>
-      <c r="B30" s="28">
+      <c r="B30" s="18">
         <v>43123</v>
       </c>
-      <c r="C30" s="23">
+      <c r="C30" s="28">
         <v>43124</v>
       </c>
       <c r="D30" s="23">
@@ -2634,118 +2829,118 @@
       <c r="A31" s="31" t="s">
         <v>157</v>
       </c>
-      <c r="B31" s="34" t="s">
-        <v>226</v>
-      </c>
-      <c r="C31" s="32" t="s">
+      <c r="B31" s="27" t="s">
+        <v>224</v>
+      </c>
+      <c r="C31" s="34" t="s">
+        <v>225</v>
+      </c>
+      <c r="D31" s="32" t="s">
+        <v>163</v>
+      </c>
+      <c r="E31" s="32" t="s">
         <v>164</v>
       </c>
-      <c r="D31" s="32" t="s">
+      <c r="F31" s="32" t="s">
         <v>165</v>
       </c>
-      <c r="E31" s="32" t="s">
+      <c r="G31" s="32" t="s">
         <v>166</v>
       </c>
-      <c r="F31" s="32" t="s">
+      <c r="H31" s="32" t="s">
         <v>167</v>
       </c>
-      <c r="G31" s="32" t="s">
+      <c r="I31" s="32" t="s">
         <v>168</v>
       </c>
-      <c r="H31" s="32" t="s">
+      <c r="J31" s="32" t="s">
         <v>169</v>
       </c>
-      <c r="I31" s="32" t="s">
+      <c r="K31" s="32" t="s">
         <v>170</v>
       </c>
-      <c r="J31" s="32" t="s">
+      <c r="L31" s="32" t="s">
         <v>171</v>
       </c>
-      <c r="K31" s="32" t="s">
-        <v>163</v>
-      </c>
-      <c r="L31" s="32" t="s">
-        <v>164</v>
-      </c>
       <c r="M31" s="32" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="N31" s="32" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="O31" s="32" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="P31" s="32" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="Q31" s="32" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="R31" s="32" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="S31" s="32" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
     </row>
     <row r="32" spans="1:19" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="31" t="s">
         <v>156</v>
       </c>
-      <c r="B32" s="34" t="s">
+      <c r="B32" s="27" t="s">
+        <v>226</v>
+      </c>
+      <c r="C32" s="34" t="s">
+        <v>289</v>
+      </c>
+      <c r="D32" s="32" t="s">
         <v>227</v>
       </c>
-      <c r="C32" s="32" t="s">
-        <v>164</v>
-      </c>
-      <c r="D32" s="32" t="s">
-        <v>165</v>
-      </c>
       <c r="E32" s="32" t="s">
-        <v>166</v>
+        <v>228</v>
       </c>
       <c r="F32" s="32" t="s">
-        <v>167</v>
+        <v>229</v>
       </c>
       <c r="G32" s="32" t="s">
-        <v>168</v>
+        <v>230</v>
       </c>
       <c r="H32" s="32" t="s">
-        <v>169</v>
+        <v>231</v>
       </c>
       <c r="I32" s="32" t="s">
-        <v>170</v>
+        <v>232</v>
       </c>
       <c r="J32" s="32" t="s">
-        <v>171</v>
+        <v>233</v>
       </c>
       <c r="K32" s="32" t="s">
-        <v>163</v>
+        <v>234</v>
       </c>
       <c r="L32" s="32" t="s">
-        <v>164</v>
+        <v>235</v>
       </c>
       <c r="M32" s="32" t="s">
-        <v>165</v>
+        <v>236</v>
       </c>
       <c r="N32" s="32" t="s">
-        <v>166</v>
+        <v>237</v>
       </c>
       <c r="O32" s="32" t="s">
-        <v>167</v>
+        <v>238</v>
       </c>
       <c r="P32" s="32" t="s">
-        <v>168</v>
+        <v>239</v>
       </c>
       <c r="Q32" s="32" t="s">
-        <v>169</v>
+        <v>240</v>
       </c>
       <c r="R32" s="32" t="s">
-        <v>170</v>
+        <v>241</v>
       </c>
       <c r="S32" s="32" t="s">
-        <v>171</v>
+        <v>242</v>
       </c>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.25">
@@ -2810,58 +3005,58 @@
         <v>155</v>
       </c>
       <c r="B36" s="32" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="C36" s="32" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="D36" s="32" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="E36" s="32" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="F36" s="32" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="G36" s="32" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="H36" s="32" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="I36" s="32" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="J36" s="32" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="K36" s="32" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="L36" s="32" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="M36" s="32" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="N36" s="32" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
       <c r="O36" s="32" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="P36" s="32" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="Q36" s="32" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="R36" s="32" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="S36" s="32" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
     </row>
     <row r="37" spans="1:19" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2869,58 +3064,58 @@
         <v>156</v>
       </c>
       <c r="B37" s="32" t="s">
-        <v>172</v>
+        <v>252</v>
       </c>
       <c r="C37" s="32" t="s">
-        <v>173</v>
+        <v>253</v>
       </c>
       <c r="D37" s="32" t="s">
-        <v>174</v>
+        <v>254</v>
       </c>
       <c r="E37" s="32" t="s">
-        <v>175</v>
+        <v>255</v>
       </c>
       <c r="F37" s="32" t="s">
-        <v>176</v>
+        <v>256</v>
       </c>
       <c r="G37" s="32" t="s">
-        <v>177</v>
+        <v>257</v>
       </c>
       <c r="H37" s="32" t="s">
-        <v>178</v>
+        <v>258</v>
       </c>
       <c r="I37" s="32" t="s">
-        <v>179</v>
+        <v>259</v>
       </c>
       <c r="J37" s="32" t="s">
-        <v>180</v>
+        <v>260</v>
       </c>
       <c r="K37" s="32" t="s">
-        <v>181</v>
+        <v>261</v>
       </c>
       <c r="L37" s="32" t="s">
-        <v>182</v>
+        <v>262</v>
       </c>
       <c r="M37" s="32" t="s">
-        <v>183</v>
+        <v>263</v>
       </c>
       <c r="N37" s="32" t="s">
-        <v>184</v>
+        <v>264</v>
       </c>
       <c r="O37" s="32" t="s">
-        <v>185</v>
+        <v>265</v>
       </c>
       <c r="P37" s="32" t="s">
-        <v>186</v>
+        <v>266</v>
       </c>
       <c r="Q37" s="32" t="s">
-        <v>187</v>
+        <v>267</v>
       </c>
       <c r="R37" s="32" t="s">
-        <v>188</v>
+        <v>268</v>
       </c>
       <c r="S37" s="32" t="s">
-        <v>189</v>
+        <v>269</v>
       </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.25">
@@ -2985,58 +3180,58 @@
         <v>155</v>
       </c>
       <c r="B41" s="32" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="C41" s="32" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="D41" s="32" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="E41" s="32" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="F41" s="32" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="G41" s="32" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="H41" s="32" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="I41" s="32" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
       <c r="J41" s="32" t="s">
-        <v>199</v>
+        <v>206</v>
       </c>
       <c r="K41" s="32" t="s">
-        <v>200</v>
+        <v>243</v>
       </c>
       <c r="L41" s="32" t="s">
-        <v>201</v>
+        <v>244</v>
       </c>
       <c r="M41" s="32" t="s">
-        <v>202</v>
+        <v>245</v>
       </c>
       <c r="N41" s="32" t="s">
-        <v>203</v>
+        <v>246</v>
       </c>
       <c r="O41" s="32" t="s">
-        <v>204</v>
+        <v>247</v>
       </c>
       <c r="P41" s="32" t="s">
-        <v>205</v>
+        <v>248</v>
       </c>
       <c r="Q41" s="32" t="s">
-        <v>206</v>
+        <v>249</v>
       </c>
       <c r="R41" s="32" t="s">
-        <v>207</v>
+        <v>250</v>
       </c>
       <c r="S41" s="32" t="s">
-        <v>208</v>
+        <v>251</v>
       </c>
     </row>
     <row r="42" spans="1:19" ht="75" x14ac:dyDescent="0.25">
@@ -3044,58 +3239,66 @@
         <v>156</v>
       </c>
       <c r="B42" s="32" t="s">
-        <v>190</v>
+        <v>270</v>
       </c>
       <c r="C42" s="32" t="s">
-        <v>191</v>
+        <v>271</v>
       </c>
       <c r="D42" s="32" t="s">
-        <v>192</v>
+        <v>272</v>
       </c>
       <c r="E42" s="32" t="s">
-        <v>193</v>
+        <v>273</v>
       </c>
       <c r="F42" s="32" t="s">
-        <v>194</v>
+        <v>274</v>
       </c>
       <c r="G42" s="32" t="s">
+        <v>275</v>
+      </c>
+      <c r="H42" s="32" t="s">
+        <v>276</v>
+      </c>
+      <c r="I42" s="32" t="s">
+        <v>277</v>
+      </c>
+      <c r="J42" s="32" t="s">
+        <v>278</v>
+      </c>
+      <c r="K42" s="32" t="s">
+        <v>279</v>
+      </c>
+      <c r="L42" s="32" t="s">
+        <v>280</v>
+      </c>
+      <c r="M42" s="32" t="s">
+        <v>281</v>
+      </c>
+      <c r="N42" s="32" t="s">
+        <v>282</v>
+      </c>
+      <c r="O42" s="32" t="s">
+        <v>283</v>
+      </c>
+      <c r="P42" s="32" t="s">
+        <v>284</v>
+      </c>
+      <c r="Q42" s="32" t="s">
+        <v>285</v>
+      </c>
+      <c r="R42" s="32" t="s">
+        <v>286</v>
+      </c>
+      <c r="S42" s="32" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+      <c r="L46" s="32" t="s">
         <v>195</v>
       </c>
-      <c r="H42" s="32" t="s">
-        <v>196</v>
-      </c>
-      <c r="I42" s="32" t="s">
-        <v>197</v>
-      </c>
-      <c r="J42" s="35" t="s">
-        <v>24</v>
-      </c>
-      <c r="K42" s="35" t="s">
-        <v>24</v>
-      </c>
-      <c r="L42" s="35" t="s">
-        <v>24</v>
-      </c>
-      <c r="M42" s="35" t="s">
-        <v>24</v>
-      </c>
-      <c r="N42" s="35" t="s">
-        <v>24</v>
-      </c>
-      <c r="O42" s="35" t="s">
-        <v>24</v>
-      </c>
-      <c r="P42" s="35" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q42" s="35" t="s">
-        <v>24</v>
-      </c>
-      <c r="R42" s="35" t="s">
-        <v>24</v>
-      </c>
-      <c r="S42" s="35" t="s">
-        <v>24</v>
+      <c r="M46" s="35" t="s">
+        <v>288</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes in the plan
</commit_message>
<xml_diff>
--- a/PLAN_Workflow.xlsx
+++ b/PLAN_Workflow.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="373">
   <si>
     <t>Book "Refactoring"
 (read)</t>
@@ -1210,10 +1210,6 @@
   </si>
   <si>
     <t xml:space="preserve">
-(291-300)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
 (301-310)</t>
   </si>
   <si>
@@ -1388,6 +1384,17 @@
   <si>
     <t>239
 (231-240)</t>
+  </si>
+  <si>
+    <t>272
+(271-280)</t>
+  </si>
+  <si>
+    <t>Pro C# 7: With .NET and .NET Core 8th ed. Edition / PRO Git</t>
+  </si>
+  <si>
+    <t>295
+(291-300)</t>
   </si>
 </sst>
 </file>
@@ -1666,7 +1673,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="6" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1793,6 +1800,7 @@
     <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2136,8 +2144,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:W78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K64" sqref="K64"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L69" sqref="L69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4320,12 +4328,12 @@
       <c r="I60" s="3" t="s">
         <v>305</v>
       </c>
-      <c r="J60" s="56" t="s">
+      <c r="J60" s="57" t="s">
         <v>306</v>
       </c>
-      <c r="K60" s="57"/>
-      <c r="L60" s="57"/>
-      <c r="M60" s="58"/>
+      <c r="K60" s="58"/>
+      <c r="L60" s="58"/>
+      <c r="M60" s="59"/>
       <c r="N60" s="16" t="s">
         <v>307</v>
       </c>
@@ -4412,34 +4420,34 @@
       <c r="J63" s="13">
         <v>43300</v>
       </c>
-      <c r="K63" s="53">
+      <c r="K63" s="13">
         <v>43301</v>
       </c>
-      <c r="L63" s="48">
+      <c r="L63" s="13">
         <v>43304</v>
       </c>
-      <c r="M63" s="48">
+      <c r="M63" s="13">
         <v>43305</v>
       </c>
-      <c r="N63" s="48">
+      <c r="N63" s="13">
         <v>43306</v>
       </c>
-      <c r="O63" s="48">
+      <c r="O63" s="13">
         <v>43307</v>
       </c>
-      <c r="P63" s="48">
+      <c r="P63" s="13">
         <v>43308</v>
       </c>
-      <c r="Q63" s="48">
+      <c r="Q63" s="13">
         <v>43311</v>
       </c>
-      <c r="R63" s="48">
+      <c r="R63" s="13">
         <v>43312</v>
       </c>
-      <c r="S63" s="48">
+      <c r="S63" s="13">
         <v>43313</v>
       </c>
-      <c r="T63" s="48">
+      <c r="T63" s="53">
         <v>43314</v>
       </c>
       <c r="U63" s="48">
@@ -4466,46 +4474,40 @@
       <c r="I64" s="3" t="s">
         <v>310</v>
       </c>
-      <c r="J64" s="52" t="s">
+      <c r="J64" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="K64" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="L64" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="M64" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="N64" s="56"/>
+      <c r="O64" s="56"/>
+      <c r="P64" s="56"/>
+      <c r="Q64" s="3" t="s">
         <v>370</v>
       </c>
-      <c r="K64" s="6" t="s">
-        <v>311</v>
-      </c>
-      <c r="L64" s="6" t="s">
-        <v>189</v>
-      </c>
-      <c r="M64" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="N64" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="O64" s="6" t="s">
+      <c r="R64" s="3" t="s">
         <v>312</v>
       </c>
-      <c r="P64" s="6" t="s">
+      <c r="S64" s="52" t="s">
+        <v>372</v>
+      </c>
+      <c r="T64" s="6" t="s">
         <v>313</v>
       </c>
-      <c r="Q64" s="6" t="s">
+      <c r="U64" s="6" t="s">
         <v>314</v>
-      </c>
-      <c r="R64" s="6" t="s">
-        <v>315</v>
-      </c>
-      <c r="S64" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="T64" s="6" t="s">
-        <v>316</v>
-      </c>
-      <c r="U64" s="6" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="65" spans="1:23" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="19" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B65" s="20"/>
       <c r="C65" s="20"/>
@@ -4514,44 +4516,28 @@
       <c r="F65" s="20"/>
       <c r="G65" s="20"/>
       <c r="H65" s="20"/>
-      <c r="I65" s="52" t="s">
+      <c r="I65" s="20"/>
+      <c r="J65" s="20"/>
+      <c r="K65" s="20"/>
+      <c r="L65" s="20"/>
+      <c r="M65" s="20"/>
+      <c r="N65" s="20"/>
+      <c r="O65" s="20"/>
+      <c r="P65" s="20"/>
+      <c r="Q65" s="52" t="s">
         <v>245</v>
       </c>
-      <c r="J65" s="6" t="s">
+      <c r="R65" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="K65" s="6" t="s">
+      <c r="S65" s="6" t="s">
         <v>263</v>
       </c>
-      <c r="L65" s="6" t="s">
+      <c r="T65" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="M65" s="6" t="s">
+      <c r="U65" s="6" t="s">
         <v>265</v>
-      </c>
-      <c r="N65" s="6" t="s">
-        <v>266</v>
-      </c>
-      <c r="O65" s="6" t="s">
-        <v>267</v>
-      </c>
-      <c r="P65" s="6" t="s">
-        <v>268</v>
-      </c>
-      <c r="Q65" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="R65" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="S65" s="6" t="s">
-        <v>271</v>
-      </c>
-      <c r="T65" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="U65" s="6" t="s">
-        <v>318</v>
       </c>
       <c r="V65" s="31"/>
       <c r="W65" s="31"/>
@@ -4673,92 +4659,108 @@
     </row>
     <row r="69" spans="1:23" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="B69" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="C69" s="6" t="s">
+        <v>315</v>
+      </c>
+      <c r="D69" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="E69" s="6" t="s">
         <v>319</v>
       </c>
-      <c r="B69" s="6" t="s">
+      <c r="F69" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="G69" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="H69" s="54" t="s">
         <v>320</v>
       </c>
-      <c r="C69" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="D69" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="E69" s="54" t="s">
+      <c r="I69" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="F69" s="6" t="s">
+      <c r="J69" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="G69" s="6" t="s">
+      <c r="K69" s="6" t="s">
         <v>323</v>
       </c>
-      <c r="H69" s="6" t="s">
+      <c r="L69" s="6" t="s">
         <v>324</v>
       </c>
-      <c r="I69" s="6" t="s">
+      <c r="M69" s="6" t="s">
         <v>325</v>
       </c>
-      <c r="J69" s="6" t="s">
+      <c r="N69" s="6" t="s">
         <v>326</v>
       </c>
-      <c r="K69" s="6" t="s">
+      <c r="O69" s="6" t="s">
         <v>327</v>
       </c>
-      <c r="L69" s="6" t="s">
+      <c r="P69" s="6" t="s">
         <v>328</v>
       </c>
-      <c r="M69" s="6" t="s">
+      <c r="Q69" s="6" t="s">
         <v>329</v>
       </c>
-      <c r="N69" s="6" t="s">
+      <c r="R69" s="6" t="s">
         <v>330</v>
       </c>
-      <c r="O69" s="6" t="s">
+      <c r="S69" s="6" t="s">
         <v>331</v>
       </c>
-      <c r="P69" s="6" t="s">
+      <c r="T69" s="6" t="s">
         <v>332</v>
       </c>
-      <c r="Q69" s="6" t="s">
+      <c r="U69" s="6" t="s">
         <v>333</v>
-      </c>
-      <c r="R69" s="6" t="s">
-        <v>334</v>
-      </c>
-      <c r="S69" s="6" t="s">
-        <v>335</v>
-      </c>
-      <c r="T69" s="6" t="s">
-        <v>336</v>
-      </c>
-      <c r="U69" s="6" t="s">
-        <v>337</v>
       </c>
       <c r="V69" s="31"/>
       <c r="W69" s="31"/>
     </row>
     <row r="70" spans="1:23" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="19" t="s">
+        <v>316</v>
+      </c>
+      <c r="B70" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="C70" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="D70" s="6" t="s">
+        <v>268</v>
+      </c>
+      <c r="E70" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="F70" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="G70" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="H70" s="6" t="s">
+        <v>298</v>
+      </c>
+      <c r="I70" s="6" t="s">
         <v>317</v>
       </c>
-      <c r="B70" s="59" t="s">
+      <c r="J70" s="60" t="s">
         <v>306</v>
       </c>
-      <c r="C70" s="60"/>
-      <c r="D70" s="60"/>
-      <c r="E70" s="61"/>
-      <c r="F70" s="24" t="s">
-        <v>338</v>
-      </c>
-      <c r="G70" s="6"/>
-      <c r="H70" s="6"/>
-      <c r="I70" s="6"/>
-      <c r="J70" s="6"/>
-      <c r="K70" s="6"/>
-      <c r="L70" s="6"/>
-      <c r="M70" s="6"/>
-      <c r="N70" s="6"/>
+      <c r="K70" s="61"/>
+      <c r="L70" s="61"/>
+      <c r="M70" s="62"/>
+      <c r="N70" s="24" t="s">
+        <v>337</v>
+      </c>
       <c r="O70" s="6"/>
       <c r="P70" s="6"/>
       <c r="Q70" s="6"/>
@@ -4889,64 +4891,64 @@
         <v>186</v>
       </c>
       <c r="B74" s="6" t="s">
+        <v>334</v>
+      </c>
+      <c r="C74" s="6" t="s">
+        <v>335</v>
+      </c>
+      <c r="D74" s="6" t="s">
+        <v>336</v>
+      </c>
+      <c r="E74" s="6" t="s">
+        <v>338</v>
+      </c>
+      <c r="F74" s="6" t="s">
         <v>339</v>
       </c>
-      <c r="C74" s="6" t="s">
+      <c r="G74" s="6" t="s">
         <v>340</v>
       </c>
-      <c r="D74" s="6" t="s">
+      <c r="H74" s="6" t="s">
         <v>341</v>
       </c>
-      <c r="E74" s="6" t="s">
+      <c r="I74" s="6" t="s">
         <v>342</v>
       </c>
-      <c r="F74" s="6" t="s">
+      <c r="J74" s="6" t="s">
         <v>343</v>
       </c>
-      <c r="G74" s="6" t="s">
+      <c r="K74" s="6" t="s">
         <v>344</v>
       </c>
-      <c r="H74" s="6" t="s">
+      <c r="L74" s="6" t="s">
         <v>345</v>
       </c>
-      <c r="I74" s="6" t="s">
+      <c r="M74" s="6" t="s">
         <v>346</v>
       </c>
-      <c r="J74" s="6" t="s">
+      <c r="N74" s="6" t="s">
         <v>347</v>
       </c>
-      <c r="K74" s="6" t="s">
+      <c r="O74" s="6" t="s">
         <v>348</v>
       </c>
-      <c r="L74" s="6" t="s">
+      <c r="P74" s="6" t="s">
         <v>349</v>
       </c>
-      <c r="M74" s="6" t="s">
+      <c r="Q74" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="N74" s="6" t="s">
+      <c r="R74" s="6" t="s">
         <v>351</v>
       </c>
-      <c r="O74" s="6" t="s">
+      <c r="S74" s="6" t="s">
         <v>352</v>
       </c>
-      <c r="P74" s="6" t="s">
+      <c r="T74" s="6" t="s">
         <v>353</v>
       </c>
-      <c r="Q74" s="6" t="s">
+      <c r="U74" s="6" t="s">
         <v>354</v>
-      </c>
-      <c r="R74" s="6" t="s">
-        <v>355</v>
-      </c>
-      <c r="S74" s="6" t="s">
-        <v>356</v>
-      </c>
-      <c r="T74" s="6" t="s">
-        <v>357</v>
-      </c>
-      <c r="U74" s="6" t="s">
-        <v>358</v>
       </c>
       <c r="V74" s="31"/>
       <c r="W74" s="31"/>
@@ -5002,45 +5004,51 @@
     </row>
     <row r="78" spans="1:23" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
-        <v>186</v>
+        <v>371</v>
       </c>
       <c r="B78" s="6" t="s">
+        <v>355</v>
+      </c>
+      <c r="C78" s="6" t="s">
+        <v>356</v>
+      </c>
+      <c r="D78" s="6" t="s">
+        <v>357</v>
+      </c>
+      <c r="E78" s="6" t="s">
+        <v>358</v>
+      </c>
+      <c r="F78" s="6" t="s">
         <v>359</v>
       </c>
-      <c r="C78" s="6" t="s">
+      <c r="G78" s="6" t="s">
         <v>360</v>
       </c>
-      <c r="D78" s="6" t="s">
+      <c r="H78" s="6" t="s">
         <v>361</v>
       </c>
-      <c r="E78" s="6" t="s">
+      <c r="I78" s="6" t="s">
         <v>362</v>
       </c>
-      <c r="F78" s="6" t="s">
+      <c r="J78" s="6" t="s">
         <v>363</v>
       </c>
-      <c r="G78" s="6" t="s">
+      <c r="K78" s="6" t="s">
         <v>364</v>
       </c>
-      <c r="H78" s="6" t="s">
+      <c r="L78" s="6" t="s">
         <v>365</v>
       </c>
-      <c r="I78" s="6" t="s">
+      <c r="M78" s="6" t="s">
         <v>366</v>
       </c>
-      <c r="J78" s="6" t="s">
+      <c r="N78" s="6" t="s">
         <v>367</v>
       </c>
-      <c r="K78" s="6" t="s">
+      <c r="O78" s="6" t="s">
         <v>368</v>
       </c>
-      <c r="L78" s="6" t="s">
-        <v>369</v>
-      </c>
-      <c r="M78" s="55"/>
-      <c r="N78" s="6"/>
-      <c r="O78" s="6"/>
-      <c r="P78" s="6"/>
+      <c r="P78" s="55"/>
       <c r="Q78" s="6"/>
       <c r="R78" s="6"/>
       <c r="S78" s="6"/>
@@ -5052,7 +5060,7 @@
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="J60:M60"/>
-    <mergeCell ref="B70:E70"/>
+    <mergeCell ref="J70:M70"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>